<commit_message>
updated lady gaga valve controller parts list to change 4.7uF capacitor to 2.2uF capacitor, because no 25V 4.7uF caps are available in an 0603 package.  created order for digikey
</commit_message>
<xml_diff>
--- a/circuit boards/lady gaga v2 valve controller/parts list.xlsx
+++ b/circuit boards/lady gaga v2 valve controller/parts list.xlsx
@@ -48,9 +48,6 @@
     <t>C2,C5, C9, C10, C11, C14, C15, C17</t>
   </si>
   <si>
-    <t>4.7 uF 0603 Cap</t>
-  </si>
-  <si>
     <t>for fast valve switching</t>
   </si>
   <si>
@@ -364,6 +361,9 @@
   </si>
   <si>
     <t>X1103-ND</t>
+  </si>
+  <si>
+    <t>2.2 uF 0603 Cap</t>
   </si>
 </sst>
 </file>
@@ -716,7 +716,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,18 +765,18 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" t="s">
         <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -784,10 +784,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -795,130 +795,130 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
         <v>23</v>
-      </c>
-      <c r="E9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" t="s">
+      <c r="E10" t="s">
         <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
         <v>26</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>28</v>
-      </c>
-      <c r="E11" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
         <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
         <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" t="s">
         <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
         <v>40</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" t="s">
         <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
         <v>45</v>
-      </c>
-      <c r="B16" t="s">
-        <v>46</v>
       </c>
       <c r="C16">
         <v>15244745</v>
@@ -927,65 +927,65 @@
         <v>15244745</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
         <v>48</v>
       </c>
-      <c r="B17" t="s">
+      <c r="E17" t="s">
         <v>49</v>
-      </c>
-      <c r="E17" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
         <v>51</v>
       </c>
-      <c r="B18" t="s">
+      <c r="E18" t="s">
         <v>52</v>
-      </c>
-      <c r="E18" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
         <v>54</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>55</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>56</v>
       </c>
-      <c r="D19" t="s">
-        <v>57</v>
-      </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
         <v>58</v>
       </c>
-      <c r="B20" t="s">
-        <v>59</v>
-      </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" t="s">
         <v>60</v>
-      </c>
-      <c r="B21" t="s">
-        <v>61</v>
       </c>
       <c r="E21" t="s">
         <v>8</v>
@@ -993,66 +993,66 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
         <v>62</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>63</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>64</v>
       </c>
-      <c r="D22" t="s">
-        <v>65</v>
-      </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" t="s">
         <v>66</v>
       </c>
-      <c r="B23" t="s">
-        <v>67</v>
-      </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" t="s">
         <v>68</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>69</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>70</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>71</v>
-      </c>
-      <c r="E24" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" t="s">
         <v>73</v>
       </c>
-      <c r="B25" t="s">
+      <c r="E25" t="s">
         <v>74</v>
-      </c>
-      <c r="E25" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E26" t="s">
         <v>8</v>
@@ -1060,104 +1060,104 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" t="s">
         <v>77</v>
       </c>
-      <c r="B27" t="s">
+      <c r="E27" t="s">
         <v>78</v>
-      </c>
-      <c r="E27" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
         <v>80</v>
       </c>
-      <c r="B28" t="s">
-        <v>81</v>
-      </c>
       <c r="E28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" t="s">
         <v>82</v>
       </c>
-      <c r="B29" t="s">
-        <v>83</v>
-      </c>
       <c r="E29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" t="s">
         <v>84</v>
       </c>
-      <c r="B30" t="s">
-        <v>85</v>
-      </c>
       <c r="E30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" t="s">
         <v>87</v>
       </c>
-      <c r="B32" t="s">
-        <v>88</v>
-      </c>
       <c r="E32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" t="s">
         <v>90</v>
       </c>
-      <c r="B33" t="s">
-        <v>91</v>
-      </c>
       <c r="E33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" t="s">
         <v>92</v>
       </c>
-      <c r="B34" t="s">
-        <v>93</v>
-      </c>
       <c r="E34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" t="s">
         <v>94</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>95</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>96</v>
-      </c>
-      <c r="D35" t="s">
-        <v>97</v>
       </c>
       <c r="E35" t="s">
         <v>8</v>
@@ -1165,75 +1165,75 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
         <v>98</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>99</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>100</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>101</v>
-      </c>
-      <c r="E36" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" t="s">
         <v>103</v>
       </c>
-      <c r="B37" t="s">
-        <v>105</v>
-      </c>
-      <c r="C37" t="s">
-        <v>104</v>
-      </c>
       <c r="E37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" t="s">
         <v>106</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>107</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>108</v>
       </c>
-      <c r="D38" t="s">
-        <v>109</v>
-      </c>
       <c r="E38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" t="s">
         <v>110</v>
-      </c>
-      <c r="B39" t="s">
-        <v>111</v>
       </c>
       <c r="C39">
         <v>7805</v>
       </c>
       <c r="E39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>112</v>
+      </c>
+      <c r="B40" t="s">
         <v>113</v>
       </c>
-      <c r="B40" t="s">
+      <c r="D40" t="s">
         <v>114</v>
-      </c>
-      <c r="D40" t="s">
-        <v>115</v>
       </c>
       <c r="E40" t="s">
         <v>8</v>

</xml_diff>